<commit_message>
Added Lab 3 & finalized HW2
</commit_message>
<xml_diff>
--- a/Assignments/Assignment2(Sorting)/Delevierable PDF/Tables.xlsx
+++ b/Assignments/Assignment2(Sorting)/Delevierable PDF/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamel\Desktop\Fall 2019\Algo\Assignments\Assignment2(Sorting)\Delevierable PDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B864143-23F9-4E97-A52A-7B4ACC24A2B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E0A356-0073-4CF1-81CB-CD1D62D9E52D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="3">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -3128,25 +3128,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.2152</c:v>
+                  <c:v>6.4299999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0547</c:v>
+                  <c:v>0.32029999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3567999999999998</c:v>
+                  <c:v>0.67720000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.535600000000001</c:v>
+                  <c:v>3.8289</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.387799999999999</c:v>
+                  <c:v>5.8581000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.081</c:v>
+                  <c:v>7.7218</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.998</c:v>
+                  <c:v>43.8386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3605,25 +3605,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.3399999999999999E-2</c:v>
+                  <c:v>5.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15379999999999999</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3034</c:v>
+                  <c:v>0.21429999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5404</c:v>
+                  <c:v>0.63029999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2463000000000002</c:v>
+                  <c:v>0.73870000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2794999999999996</c:v>
+                  <c:v>1.452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.0504</c:v>
+                  <c:v>3.4165000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3888,6 +3888,1238 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Selection Unsorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3515999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.963899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.482600000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2101.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4408.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7515.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180630</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-594D-4268-A9D5-3F193B807AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Quick Unsorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.2243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53059999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2972000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7604000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.587199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.988799999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-594D-4268-A9D5-3F193B807AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Merge Unsorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.96560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2362000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9521999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.588800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.8721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.832100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>147.952</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-594D-4268-A9D5-3F193B807AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Insertion Unsorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.66390000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.6584</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.1479</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>578.06399999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>910.52099999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1595.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41462.699999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-594D-4268-A9D5-3F193B807AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Hybrid Unsorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.4299999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32029999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8289</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8581000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7218</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.8386</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-594D-4268-A9D5-3F193B807AF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Selection Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.4491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.9513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.106900000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1624.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3744.49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7285.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-070E-46AE-9BFB-BE37B3142F5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Quick Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.895099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.500599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1065.47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2539.9499999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4129.7299999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98941.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-070E-46AE-9BFB-BE37B3142F5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Merge Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.37680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5760000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1514000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.4602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.5275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.4298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101.288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-070E-46AE-9BFB-BE37B3142F5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Insertion Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1246</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53610000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-070E-46AE-9BFB-BE37B3142F5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Hybrid Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63029999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73870000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.452</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4165000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-070E-46AE-9BFB-BE37B3142F5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="344250160"/>
+        <c:axId val="344250488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="344250160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344250488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="344250488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344250160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4252,6 +5484,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7865,6 +9137,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8420,16 +10208,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8497,16 +10285,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1287780</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8574,16 +10362,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8651,16 +10439,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8680,6 +10468,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1474968</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>547315</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>144117</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F306807-2535-483C-856B-B17E4334DA02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9101,7 +10930,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9249,7 +11078,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B1" sqref="B1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9397,7 +11226,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B1" sqref="B1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9544,8 +11373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768247BF-C564-44A7-9E1F-45BA3B7F38FE}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9567,7 +11396,7 @@
         <v>1000</v>
       </c>
       <c r="B2" s="1">
-        <v>0.2152</v>
+        <v>6.4299999999999996E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9575,7 +11404,7 @@
         <v>5000</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0547</v>
+        <v>0.32029999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9583,7 +11412,7 @@
         <v>10000</v>
       </c>
       <c r="B4" s="1">
-        <v>2.3567999999999998</v>
+        <v>0.67720000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -9591,7 +11420,7 @@
         <v>50000</v>
       </c>
       <c r="B5" s="1">
-        <v>12.535600000000001</v>
+        <v>3.8289</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -9599,7 +11428,7 @@
         <v>75000</v>
       </c>
       <c r="B6" s="1">
-        <v>16.387799999999999</v>
+        <v>5.8581000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9607,7 +11436,7 @@
         <v>100000</v>
       </c>
       <c r="B7" s="1">
-        <v>21.081</v>
+        <v>7.7218</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -9615,7 +11444,7 @@
         <v>500000</v>
       </c>
       <c r="B8" s="1">
-        <v>113.998</v>
+        <v>43.8386</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9631,7 +11460,7 @@
         <v>1000</v>
       </c>
       <c r="B10" s="1">
-        <v>3.3399999999999999E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -9639,7 +11468,7 @@
         <v>5000</v>
       </c>
       <c r="B11" s="1">
-        <v>0.15379999999999999</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9647,7 +11476,7 @@
         <v>10000</v>
       </c>
       <c r="B12" s="1">
-        <v>0.3034</v>
+        <v>0.21429999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9655,7 +11484,7 @@
         <v>50000</v>
       </c>
       <c r="B13" s="1">
-        <v>1.5404</v>
+        <v>0.63029999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -9663,7 +11492,7 @@
         <v>75000</v>
       </c>
       <c r="B14" s="1">
-        <v>2.2463000000000002</v>
+        <v>0.73870000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -9671,7 +11500,7 @@
         <v>100000</v>
       </c>
       <c r="B15" s="1">
-        <v>4.2794999999999996</v>
+        <v>1.452</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -9679,7 +11508,7 @@
         <v>500000</v>
       </c>
       <c r="B16" s="1">
-        <v>15.0504</v>
+        <v>3.4165000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -9690,12 +11519,344 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E725E6B7-4269-4047-BC96-0F33C4DCB0A6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.3515999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.2243</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.96560000000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.66390000000000005</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>22.963899999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.53059999999999996</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.2362000000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11.6584</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.32029999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>88.482600000000005</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.3026</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.9521999999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>17.1479</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.67720000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2101.61</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.2972000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>14.588800000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>578.06399999999996</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.8289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>75000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4408.1000000000004</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.7604000000000006</v>
+      </c>
+      <c r="D6" s="1">
+        <v>23.8721</v>
+      </c>
+      <c r="E6" s="1">
+        <v>910.52099999999996</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5.8581000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7515.69</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10.587199999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>28.832100000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1595.04</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7.7218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>180630</v>
+      </c>
+      <c r="C8" s="1">
+        <v>56.988799999999998</v>
+      </c>
+      <c r="D8" s="1">
+        <v>147.952</v>
+      </c>
+      <c r="E8" s="1">
+        <v>41462.699999999997</v>
+      </c>
+      <c r="F8" s="1">
+        <v>43.8386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.4491</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.37680000000000002</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11.9513</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13.895099999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>48.106900000000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44.500599999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.1514000000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.21429999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1624.62</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1065.47</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10.4602</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.1246</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.63029999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>75000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3744.49</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2539.9499999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>11.5275</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.73870000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7285.14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4129.7299999999996</v>
+      </c>
+      <c r="D15" s="1">
+        <v>20.4298</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.48349999999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>135030</v>
+      </c>
+      <c r="C16" s="1">
+        <v>98941.2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>101.288</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3.4165000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>